<commit_message>
20170803 功能微調 bug fixed
</commit_message>
<xml_diff>
--- a/templates/轉出銷倉單格式範例.xlsx
+++ b/templates/轉出銷倉單格式範例.xlsx
@@ -469,9 +469,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -492,13 +489,38 @@
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="0,0_x000d__x000a_NA_x000d__x000a_" xfId="1"/>
     <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -777,7 +799,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D1:D1048576"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -785,22 +807,22 @@
     <col min="1" max="1" width="11.5" customWidth="1"/>
     <col min="2" max="2" width="13.25" customWidth="1"/>
     <col min="3" max="3" width="6" customWidth="1"/>
-    <col min="4" max="4" width="15" style="31" customWidth="1"/>
+    <col min="4" max="4" width="15" style="30" customWidth="1"/>
     <col min="5" max="5" width="27.25" customWidth="1"/>
     <col min="6" max="6" width="12.75" customWidth="1"/>
     <col min="7" max="7" width="16.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20.25">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
@@ -810,7 +832,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="24" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -829,7 +851,7 @@
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="24" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="7" t="s">
@@ -850,7 +872,7 @@
         <v>11</v>
       </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="25" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="9" t="s">
@@ -869,7 +891,7 @@
       <c r="C5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="26" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="12" t="s">
@@ -892,7 +914,7 @@
       <c r="C6" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="27" t="s">
         <v>22</v>
       </c>
       <c r="E6" s="13" t="s">
@@ -913,7 +935,7 @@
       <c r="C7" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="28" t="s">
         <v>31</v>
       </c>
       <c r="E7" s="19"/>
@@ -930,7 +952,7 @@
       <c r="C8" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="29" t="s">
         <v>32</v>
       </c>
       <c r="E8" s="22"/>
@@ -946,6 +968,11 @@
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="A6:XFD4000">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>$G6="C2035"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
20170808 功能微調 bug fixed
</commit_message>
<xml_diff>
--- a/templates/轉出銷倉單格式範例.xlsx
+++ b/templates/轉出銷倉單格式範例.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="完整版-航空公司" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'完整版-航空公司'!$A$1:$G$96</definedName>
+  </definedNames>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -498,21 +501,7 @@
     <cellStyle name="0,0_x000d__x000a_NA_x000d__x000a_" xfId="1"/>
     <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -798,7 +787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -969,11 +958,11 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A6:XFD4000">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G6="C2035"</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="88" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>